<commit_message>
fix summary table joining
</commit_message>
<xml_diff>
--- a/Output/output_HPDB - XLSGM1218.xlsx
+++ b/Output/output_HPDB - XLSGM1218.xlsx
@@ -792,11 +792,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T2" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="U2" s="3" t="n">
-        <v>3</v>
+      <c r="T2" s="3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="U2" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V2" s="3" t="inlineStr">
         <is>
@@ -1036,11 +1040,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T3" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="U3" s="3" t="n">
-        <v>3</v>
+      <c r="T3" s="3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="U3" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V3" s="3" t="inlineStr">
         <is>
@@ -1280,11 +1288,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T4" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="U4" s="3" t="n">
-        <v>3</v>
+      <c r="T4" s="3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="U4" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V4" s="3" t="inlineStr">
         <is>
@@ -1524,11 +1536,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T5" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="U5" s="3" t="n">
-        <v>3</v>
+      <c r="T5" s="3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="U5" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V5" s="3" t="inlineStr">
         <is>
@@ -1768,11 +1784,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T6" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="U6" s="3" t="n">
-        <v>3</v>
+      <c r="T6" s="3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="U6" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V6" s="3" t="inlineStr">
         <is>
@@ -2012,11 +2032,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T7" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="U7" s="3" t="n">
-        <v>3</v>
+      <c r="T7" s="3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="U7" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V7" s="3" t="inlineStr">
         <is>
@@ -2256,11 +2280,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T8" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="U8" s="3" t="n">
-        <v>3</v>
+      <c r="T8" s="3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="U8" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V8" s="3" t="inlineStr">
         <is>
@@ -2500,11 +2528,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T9" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="U9" s="3" t="n">
-        <v>3</v>
+      <c r="T9" s="3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="U9" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V9" s="3" t="inlineStr">
         <is>
@@ -2744,11 +2776,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T10" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="U10" s="3" t="n">
-        <v>3</v>
+      <c r="T10" s="3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="U10" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V10" s="3" t="inlineStr">
         <is>
@@ -2988,11 +3024,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T11" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="U11" s="3" t="n">
-        <v>3</v>
+      <c r="T11" s="3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="U11" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V11" s="3" t="inlineStr">
         <is>
@@ -3232,11 +3272,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T12" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="U12" s="3" t="n">
-        <v>3</v>
+      <c r="T12" s="3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="U12" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V12" s="3" t="inlineStr">
         <is>
@@ -3476,11 +3520,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T13" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="U13" s="3" t="n">
-        <v>3</v>
+      <c r="T13" s="3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="U13" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V13" s="3" t="inlineStr">
         <is>
@@ -3720,11 +3768,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T14" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="U14" s="3" t="n">
-        <v>3</v>
+      <c r="T14" s="3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="U14" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V14" s="3" t="inlineStr">
         <is>
@@ -3964,11 +4016,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T15" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="U15" s="3" t="n">
-        <v>3</v>
+      <c r="T15" s="3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="U15" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V15" s="3" t="inlineStr">
         <is>
@@ -4208,11 +4264,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T16" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="U16" s="3" t="n">
-        <v>3</v>
+      <c r="T16" s="3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="U16" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V16" s="3" t="inlineStr">
         <is>
@@ -4452,11 +4512,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T17" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="U17" s="3" t="n">
-        <v>3</v>
+      <c r="T17" s="3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="U17" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V17" s="3" t="inlineStr">
         <is>
@@ -4696,11 +4760,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T18" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="U18" s="3" t="n">
-        <v>3</v>
+      <c r="T18" s="3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="U18" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V18" s="3" t="inlineStr">
         <is>
@@ -4940,11 +5008,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T19" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="U19" s="3" t="n">
-        <v>3</v>
+      <c r="T19" s="3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="U19" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V19" s="3" t="inlineStr">
         <is>
@@ -5184,11 +5256,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T20" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="U20" s="3" t="n">
-        <v>3</v>
+      <c r="T20" s="3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="U20" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V20" s="3" t="inlineStr">
         <is>
@@ -5428,11 +5504,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T21" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="U21" s="3" t="n">
-        <v>3</v>
+      <c r="T21" s="3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="U21" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V21" s="3" t="inlineStr">
         <is>
@@ -5672,11 +5752,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T22" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="U22" s="3" t="n">
-        <v>3</v>
+      <c r="T22" s="3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="U22" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V22" s="3" t="inlineStr">
         <is>
@@ -5916,11 +6000,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T23" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="U23" s="3" t="n">
-        <v>3</v>
+      <c r="T23" s="3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="U23" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V23" s="3" t="inlineStr">
         <is>
@@ -6160,11 +6248,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T24" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="U24" s="3" t="n">
-        <v>3</v>
+      <c r="T24" s="3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="U24" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V24" s="3" t="inlineStr">
         <is>
@@ -6404,11 +6496,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T25" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="U25" s="3" t="n">
-        <v>3</v>
+      <c r="T25" s="3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="U25" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V25" s="3" t="inlineStr">
         <is>
@@ -6648,11 +6744,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T26" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="U26" s="3" t="n">
-        <v>3</v>
+      <c r="T26" s="3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="U26" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V26" s="3" t="inlineStr">
         <is>
@@ -6892,11 +6992,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T27" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="U27" s="3" t="n">
-        <v>3</v>
+      <c r="T27" s="3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="U27" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V27" s="3" t="inlineStr">
         <is>
@@ -7136,11 +7240,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T28" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="U28" s="3" t="n">
-        <v>3</v>
+      <c r="T28" s="3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="U28" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V28" s="3" t="inlineStr">
         <is>
@@ -7380,11 +7488,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T29" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="U29" s="3" t="n">
-        <v>3</v>
+      <c r="T29" s="3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="U29" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V29" s="3" t="inlineStr">
         <is>
@@ -7624,11 +7736,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T30" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="U30" s="3" t="n">
-        <v>3</v>
+      <c r="T30" s="3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="U30" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V30" s="3" t="inlineStr">
         <is>
@@ -7868,11 +7984,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T31" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="U31" s="3" t="n">
-        <v>3</v>
+      <c r="T31" s="3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="U31" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V31" s="3" t="inlineStr">
         <is>
@@ -8112,11 +8232,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T32" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="U32" s="3" t="n">
-        <v>3</v>
+      <c r="T32" s="3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="U32" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V32" s="3" t="inlineStr">
         <is>
@@ -8356,11 +8480,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T33" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="U33" s="3" t="n">
-        <v>3</v>
+      <c r="T33" s="3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="U33" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V33" s="3" t="inlineStr">
         <is>
@@ -8600,11 +8728,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T34" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="U34" s="3" t="n">
-        <v>3</v>
+      <c r="T34" s="3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="U34" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V34" s="3" t="inlineStr">
         <is>
@@ -8844,11 +8976,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T35" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="U35" s="3" t="n">
-        <v>3</v>
+      <c r="T35" s="3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="U35" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V35" s="3" t="inlineStr">
         <is>
@@ -9088,11 +9224,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T36" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="U36" s="3" t="n">
-        <v>3</v>
+      <c r="T36" s="3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="U36" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V36" s="3" t="inlineStr">
         <is>
@@ -9332,11 +9472,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T37" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="U37" s="3" t="n">
-        <v>3</v>
+      <c r="T37" s="3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="U37" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V37" s="3" t="inlineStr">
         <is>
@@ -9576,11 +9720,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T38" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="U38" s="3" t="n">
-        <v>3</v>
+      <c r="T38" s="3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="U38" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V38" s="3" t="inlineStr">
         <is>
@@ -9820,11 +9968,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T39" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="U39" s="3" t="n">
-        <v>3</v>
+      <c r="T39" s="3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="U39" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V39" s="3" t="inlineStr">
         <is>
@@ -10064,11 +10216,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T40" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="U40" s="3" t="n">
-        <v>3</v>
+      <c r="T40" s="3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="U40" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V40" s="3" t="inlineStr">
         <is>
@@ -10308,11 +10464,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T41" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="U41" s="3" t="n">
-        <v>3</v>
+      <c r="T41" s="3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="U41" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V41" s="3" t="inlineStr">
         <is>
@@ -10552,11 +10712,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T42" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="U42" s="3" t="n">
-        <v>3</v>
+      <c r="T42" s="3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="U42" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V42" s="3" t="inlineStr">
         <is>
@@ -10796,11 +10960,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T43" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="U43" s="3" t="n">
-        <v>3</v>
+      <c r="T43" s="3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="U43" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V43" s="3" t="inlineStr">
         <is>
@@ -11040,11 +11208,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T44" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="U44" s="3" t="n">
-        <v>3</v>
+      <c r="T44" s="3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="U44" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V44" s="3" t="inlineStr">
         <is>
@@ -11284,11 +11456,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T45" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="U45" s="3" t="n">
-        <v>3</v>
+      <c r="T45" s="3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="U45" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V45" s="3" t="inlineStr">
         <is>
@@ -11528,11 +11704,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T46" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="U46" s="3" t="n">
-        <v>3</v>
+      <c r="T46" s="3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="U46" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V46" s="3" t="inlineStr">
         <is>
@@ -11772,11 +11952,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T47" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="U47" s="3" t="n">
-        <v>3</v>
+      <c r="T47" s="3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="U47" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V47" s="3" t="inlineStr">
         <is>
@@ -12016,11 +12200,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T48" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="U48" s="3" t="n">
-        <v>3</v>
+      <c r="T48" s="3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="U48" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V48" s="3" t="inlineStr">
         <is>
@@ -12260,11 +12448,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T49" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="U49" s="3" t="n">
-        <v>3</v>
+      <c r="T49" s="3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="U49" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V49" s="3" t="inlineStr">
         <is>
@@ -12504,11 +12696,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T50" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="U50" s="3" t="n">
-        <v>3</v>
+      <c r="T50" s="3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="U50" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V50" s="3" t="inlineStr">
         <is>
@@ -12748,11 +12944,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T51" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="U51" s="3" t="n">
-        <v>3</v>
+      <c r="T51" s="3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="U51" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V51" s="3" t="inlineStr">
         <is>
@@ -12992,11 +13192,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T52" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="U52" s="3" t="n">
-        <v>3</v>
+      <c r="T52" s="3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="U52" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V52" s="3" t="inlineStr">
         <is>
@@ -13236,11 +13440,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T53" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="U53" s="3" t="n">
-        <v>3</v>
+      <c r="T53" s="3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="U53" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V53" s="3" t="inlineStr">
         <is>
@@ -13480,11 +13688,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T54" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="U54" s="3" t="n">
-        <v>3</v>
+      <c r="T54" s="3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="U54" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V54" s="3" t="inlineStr">
         <is>
@@ -13724,11 +13936,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T55" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="U55" s="3" t="n">
-        <v>3</v>
+      <c r="T55" s="3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="U55" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V55" s="3" t="inlineStr">
         <is>
@@ -13968,11 +14184,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T56" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="U56" s="3" t="n">
-        <v>3</v>
+      <c r="T56" s="3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="U56" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V56" s="3" t="inlineStr">
         <is>
@@ -14212,11 +14432,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T57" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="U57" s="3" t="n">
-        <v>3</v>
+      <c r="T57" s="3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="U57" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V57" s="3" t="inlineStr">
         <is>
@@ -14456,11 +14680,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T58" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="U58" s="3" t="n">
-        <v>3</v>
+      <c r="T58" s="3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="U58" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V58" s="3" t="inlineStr">
         <is>
@@ -14700,11 +14928,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T59" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="U59" s="3" t="n">
-        <v>3</v>
+      <c r="T59" s="3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="U59" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V59" s="3" t="inlineStr">
         <is>
@@ -14944,11 +15176,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T60" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="U60" s="3" t="n">
-        <v>3</v>
+      <c r="T60" s="3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="U60" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V60" s="3" t="inlineStr">
         <is>
@@ -15188,11 +15424,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T61" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="U61" s="3" t="n">
-        <v>3</v>
+      <c r="T61" s="3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="U61" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V61" s="3" t="inlineStr">
         <is>
@@ -15432,11 +15672,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T62" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="U62" s="3" t="n">
-        <v>3</v>
+      <c r="T62" s="3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="U62" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V62" s="3" t="inlineStr">
         <is>
@@ -15676,11 +15920,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T63" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="U63" s="3" t="n">
-        <v>3</v>
+      <c r="T63" s="3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="U63" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V63" s="3" t="inlineStr">
         <is>
@@ -15920,11 +16168,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T64" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="U64" s="3" t="n">
-        <v>3</v>
+      <c r="T64" s="3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="U64" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V64" s="3" t="inlineStr">
         <is>
@@ -16164,11 +16416,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T65" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="U65" s="3" t="n">
-        <v>3</v>
+      <c r="T65" s="3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="U65" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V65" s="3" t="inlineStr">
         <is>
@@ -16408,11 +16664,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T66" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="U66" s="3" t="n">
-        <v>3</v>
+      <c r="T66" s="3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="U66" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V66" s="3" t="inlineStr">
         <is>
@@ -16652,11 +16912,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T67" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="U67" s="3" t="n">
-        <v>3</v>
+      <c r="T67" s="3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="U67" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V67" s="3" t="inlineStr">
         <is>
@@ -16896,11 +17160,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T68" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="U68" s="3" t="n">
-        <v>3</v>
+      <c r="T68" s="3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="U68" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V68" s="3" t="inlineStr">
         <is>
@@ -17140,11 +17408,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T69" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="U69" s="3" t="n">
-        <v>3</v>
+      <c r="T69" s="3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="U69" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V69" s="3" t="inlineStr">
         <is>
@@ -17384,11 +17656,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T70" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="U70" s="3" t="n">
-        <v>3</v>
+      <c r="T70" s="3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="U70" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V70" s="3" t="inlineStr">
         <is>
@@ -17628,11 +17904,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T71" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="U71" s="3" t="n">
-        <v>3</v>
+      <c r="T71" s="3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="U71" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V71" s="3" t="inlineStr">
         <is>
@@ -17872,11 +18152,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T72" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="U72" s="3" t="n">
-        <v>3</v>
+      <c r="T72" s="3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="U72" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V72" s="3" t="inlineStr">
         <is>
@@ -18116,11 +18400,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T73" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="U73" s="3" t="n">
-        <v>3</v>
+      <c r="T73" s="3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="U73" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V73" s="3" t="inlineStr">
         <is>
@@ -18360,11 +18648,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T74" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="U74" s="3" t="n">
-        <v>3</v>
+      <c r="T74" s="3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="U74" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V74" s="3" t="inlineStr">
         <is>
@@ -18604,11 +18896,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T75" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="U75" s="3" t="n">
-        <v>3</v>
+      <c r="T75" s="3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="U75" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V75" s="3" t="inlineStr">
         <is>
@@ -18848,11 +19144,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T76" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="U76" s="3" t="n">
-        <v>3</v>
+      <c r="T76" s="3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="U76" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V76" s="3" t="inlineStr">
         <is>
@@ -19092,11 +19392,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T77" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="U77" s="3" t="n">
-        <v>3</v>
+      <c r="T77" s="3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="U77" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V77" s="3" t="inlineStr">
         <is>
@@ -19336,11 +19640,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T78" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="U78" s="3" t="n">
-        <v>3</v>
+      <c r="T78" s="3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="U78" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V78" s="3" t="inlineStr">
         <is>
@@ -19580,11 +19888,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T79" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="U79" s="3" t="n">
-        <v>3</v>
+      <c r="T79" s="3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="U79" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V79" s="3" t="inlineStr">
         <is>
@@ -19824,11 +20136,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T80" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="U80" s="3" t="n">
-        <v>3</v>
+      <c r="T80" s="3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="U80" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V80" s="3" t="inlineStr">
         <is>
@@ -20068,11 +20384,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T81" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="U81" s="3" t="n">
-        <v>3</v>
+      <c r="T81" s="3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="U81" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V81" s="3" t="inlineStr">
         <is>
@@ -20312,11 +20632,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T82" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="U82" s="3" t="n">
-        <v>3</v>
+      <c r="T82" s="3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="U82" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V82" s="3" t="inlineStr">
         <is>
@@ -20556,11 +20880,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T83" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="U83" s="3" t="n">
-        <v>3</v>
+      <c r="T83" s="3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="U83" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V83" s="3" t="inlineStr">
         <is>
@@ -20800,11 +21128,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T84" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="U84" s="3" t="n">
-        <v>3</v>
+      <c r="T84" s="3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="U84" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V84" s="3" t="inlineStr">
         <is>
@@ -21044,11 +21376,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T85" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="U85" s="3" t="n">
-        <v>3</v>
+      <c r="T85" s="3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="U85" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V85" s="3" t="inlineStr">
         <is>
@@ -21288,11 +21624,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T86" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="U86" s="3" t="n">
-        <v>3</v>
+      <c r="T86" s="3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="U86" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V86" s="3" t="inlineStr">
         <is>
@@ -21532,11 +21872,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T87" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="U87" s="3" t="n">
-        <v>3</v>
+      <c r="T87" s="3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="U87" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V87" s="3" t="inlineStr">
         <is>
@@ -21776,11 +22120,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T88" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="U88" s="3" t="n">
-        <v>3</v>
+      <c r="T88" s="3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="U88" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V88" s="3" t="inlineStr">
         <is>
@@ -22020,11 +22368,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T89" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="U89" s="3" t="n">
-        <v>3</v>
+      <c r="T89" s="3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="U89" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V89" s="3" t="inlineStr">
         <is>
@@ -22264,11 +22616,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T90" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="U90" s="3" t="n">
-        <v>3</v>
+      <c r="T90" s="3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="U90" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V90" s="3" t="inlineStr">
         <is>
@@ -22508,11 +22864,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T91" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="U91" s="3" t="n">
-        <v>3</v>
+      <c r="T91" s="3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="U91" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V91" s="3" t="inlineStr">
         <is>
@@ -22752,11 +23112,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T92" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="U92" s="3" t="n">
-        <v>3</v>
+      <c r="T92" s="3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="U92" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V92" s="3" t="inlineStr">
         <is>
@@ -22996,11 +23360,15 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T93" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="U93" s="3" t="n">
-        <v>3</v>
+      <c r="T93" s="3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="U93" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="V93" s="3" t="inlineStr">
         <is>

</xml_diff>